<commit_message>
NB Reporting: - KZT Form 10 done (IFRS-9)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_10.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_10.xlsx
@@ -136,36 +136,21 @@
     <t>Изменение (гр.23-гр.22)</t>
   </si>
   <si>
-    <t>Прочие краткосрочные активы (сумма строк 2-3)</t>
-  </si>
-  <si>
     <t>Расходы будущих периодов</t>
   </si>
   <si>
     <t>Прочие краткосрочные активы</t>
   </si>
   <si>
-    <t>Прочие долгосрочные активы (сумма строк 5-10 )</t>
-  </si>
-  <si>
     <t>Инвестиции в недвижимость</t>
   </si>
   <si>
-    <t>Биологические активы</t>
-  </si>
-  <si>
-    <t>Разведочные и оценочные активы</t>
-  </si>
-  <si>
     <t>Незавершенное строительство</t>
   </si>
   <si>
     <t>Прочие долгосрочные активы</t>
   </si>
   <si>
-    <t>ВСЕГО  (сумма строк 1, 4)</t>
-  </si>
-  <si>
     <t>* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
   </si>
   <si>
@@ -188,6 +173,21 @@
   </si>
   <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>Прочие краткосрочные активы (сумма строк 2-4)</t>
+  </si>
+  <si>
+    <t>Краткосрочные авансы выданные</t>
+  </si>
+  <si>
+    <t>Долгосрочные авансы выданные</t>
+  </si>
+  <si>
+    <t>Всего  (сумма строк 1, 5)</t>
+  </si>
+  <si>
+    <t>Прочие долгосрочные активы (сумма строк 6-10)</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -626,63 +626,69 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1008,9 +1014,9 @@
   <dimension ref="A1:AA62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="H83" sqref="H83"/>
-      <selection pane="topRight" activeCell="Y19" sqref="Y19:Z19"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2593,7 +2599,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2828,7 +2834,7 @@
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B10" s="72"/>
       <c r="C10" s="72"/>
@@ -2887,13 +2893,13 @@
       <c r="AA11" s="15"/>
     </row>
     <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="67" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="74" t="s">
@@ -2927,107 +2933,107 @@
       <c r="V13" s="79"/>
       <c r="W13" s="79"/>
       <c r="X13" s="79"/>
-      <c r="Y13" s="64" t="s">
+      <c r="Y13" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="Z13" s="64" t="s">
+      <c r="Z13" s="67" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="73"/>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="64" t="s">
+      <c r="E14" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="69"/>
-      <c r="H14" s="68" t="s">
+      <c r="G14" s="64"/>
+      <c r="H14" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="69"/>
-      <c r="J14" s="68" t="s">
+      <c r="I14" s="64"/>
+      <c r="J14" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="69"/>
-      <c r="L14" s="68" t="s">
+      <c r="K14" s="64"/>
+      <c r="L14" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="69"/>
-      <c r="N14" s="68" t="s">
+      <c r="M14" s="64"/>
+      <c r="N14" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="69"/>
-      <c r="P14" s="64" t="s">
+      <c r="O14" s="64"/>
+      <c r="P14" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Q14" s="64" t="s">
+      <c r="Q14" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="R14" s="64" t="s">
+      <c r="R14" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="S14" s="64" t="s">
+      <c r="S14" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="T14" s="64" t="s">
+      <c r="T14" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="U14" s="64" t="s">
+      <c r="U14" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="V14" s="64" t="s">
+      <c r="V14" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="W14" s="64" t="s">
+      <c r="W14" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="X14" s="64" t="s">
+      <c r="X14" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="Y14" s="65"/>
-      <c r="Z14" s="65"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
     </row>
     <row r="15" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="73"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
-      <c r="U15" s="65"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="65"/>
-      <c r="X15" s="65"/>
-      <c r="Y15" s="65"/>
-      <c r="Z15" s="65"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="68"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
     </row>
     <row r="16" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="66"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="17" t="s">
         <v>20</v>
       </c>
@@ -3058,15 +3064,15 @@
       <c r="O16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="66"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="66"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="66"/>
-      <c r="X16" s="66"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="69"/>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
       <c r="Y16" s="80"/>
       <c r="Z16" s="80"/>
     </row>
@@ -3153,7 +3159,7 @@
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="21" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -3185,40 +3191,41 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
-      <c r="B19" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="18">
+      <c r="B19" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="62">
         <v>2</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="55"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="54"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="54"/>
+      <c r="Y19" s="54"/>
+      <c r="Z19" s="54"/>
+      <c r="AA19" s="26"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="18">
         <v>3</v>
@@ -3226,7 +3233,7 @@
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="25"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
@@ -3245,76 +3252,76 @@
       <c r="W20" s="24"/>
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
+      <c r="Z20" s="55"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
-      <c r="B21" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="22">
+      <c r="B21" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="18">
         <v>4</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="54"/>
-      <c r="V21" s="54"/>
-      <c r="W21" s="54"/>
-      <c r="X21" s="54"/>
-      <c r="Y21" s="54"/>
-      <c r="Z21" s="54"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
-      <c r="B22" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="18">
+      <c r="B22" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="22">
         <v>5</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="54"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="54"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23" s="18">
         <v>6</v>
@@ -3346,7 +3353,7 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="27" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C24" s="18">
         <v>7</v>
@@ -3378,7 +3385,7 @@
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="18">
         <v>8</v>
@@ -3411,7 +3418,7 @@
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26" s="18">
         <v>9</v>
@@ -3443,7 +3450,7 @@
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" s="18">
         <v>10</v>
@@ -3473,10 +3480,10 @@
       <c r="Z27" s="24"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="67"/>
+      <c r="A28" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="82"/>
       <c r="C28" s="30">
         <v>11</v>
       </c>
@@ -3512,184 +3519,184 @@
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="71"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="71"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="71"/>
+      <c r="T30" s="71"/>
+      <c r="U30" s="71"/>
+      <c r="V30" s="71"/>
+      <c r="W30" s="71"/>
+      <c r="X30" s="71"/>
+      <c r="Y30" s="71"/>
+      <c r="Z30" s="71"/>
+    </row>
+    <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+      <c r="S31" s="71"/>
+      <c r="T31" s="71"/>
+      <c r="U31" s="71"/>
+      <c r="V31" s="71"/>
+      <c r="W31" s="71"/>
+      <c r="X31" s="71"/>
+      <c r="Y31" s="71"/>
+      <c r="Z31" s="71"/>
+    </row>
+    <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="71"/>
+      <c r="S32" s="71"/>
+      <c r="T32" s="71"/>
+      <c r="U32" s="71"/>
+      <c r="V32" s="71"/>
+      <c r="W32" s="71"/>
+      <c r="X32" s="71"/>
+      <c r="Y32" s="71"/>
+      <c r="Z32" s="71"/>
+    </row>
+    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
+      <c r="S33" s="71"/>
+      <c r="T33" s="71"/>
+      <c r="U33" s="71"/>
+      <c r="V33" s="71"/>
+      <c r="W33" s="71"/>
+      <c r="X33" s="71"/>
+      <c r="Y33" s="71"/>
+      <c r="Z33" s="71"/>
+    </row>
+    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+      <c r="N34" s="71"/>
+      <c r="O34" s="71"/>
+      <c r="P34" s="71"/>
+      <c r="Q34" s="71"/>
+      <c r="R34" s="71"/>
+      <c r="S34" s="71"/>
+      <c r="T34" s="71"/>
+      <c r="U34" s="71"/>
+      <c r="V34" s="71"/>
+      <c r="W34" s="71"/>
+      <c r="X34" s="71"/>
+      <c r="Y34" s="71"/>
+      <c r="Z34" s="71"/>
+    </row>
+    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="62"/>
-      <c r="R30" s="62"/>
-      <c r="S30" s="62"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="62"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="62"/>
-      <c r="X30" s="62"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="62"/>
-    </row>
-    <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="62"/>
-      <c r="R31" s="62"/>
-      <c r="S31" s="62"/>
-      <c r="T31" s="62"/>
-      <c r="U31" s="62"/>
-      <c r="V31" s="62"/>
-      <c r="W31" s="62"/>
-      <c r="X31" s="62"/>
-      <c r="Y31" s="62"/>
-      <c r="Z31" s="62"/>
-    </row>
-    <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="62"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62"/>
-      <c r="S32" s="62"/>
-      <c r="T32" s="62"/>
-      <c r="U32" s="62"/>
-      <c r="V32" s="62"/>
-      <c r="W32" s="62"/>
-      <c r="X32" s="62"/>
-      <c r="Y32" s="62"/>
-      <c r="Z32" s="62"/>
-    </row>
-    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="62"/>
-      <c r="T33" s="62"/>
-      <c r="U33" s="62"/>
-      <c r="V33" s="62"/>
-      <c r="W33" s="62"/>
-      <c r="X33" s="62"/>
-      <c r="Y33" s="62"/>
-      <c r="Z33" s="62"/>
-    </row>
-    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="62"/>
-      <c r="S34" s="62"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
-      <c r="Y34" s="62"/>
-      <c r="Z34" s="62"/>
-    </row>
-    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="62"/>
-      <c r="S35" s="62"/>
-      <c r="T35" s="62"/>
-      <c r="U35" s="62"/>
-      <c r="V35" s="62"/>
-      <c r="W35" s="62"/>
-      <c r="X35" s="62"/>
-      <c r="Y35" s="62"/>
-      <c r="Z35" s="62"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="71"/>
+      <c r="T35" s="71"/>
+      <c r="U35" s="71"/>
+      <c r="V35" s="71"/>
+      <c r="W35" s="71"/>
+      <c r="X35" s="71"/>
+      <c r="Y35" s="71"/>
+      <c r="Z35" s="71"/>
     </row>
     <row r="36" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
       <c r="E36" s="34"/>
       <c r="F36" s="34"/>
       <c r="G36" s="35"/>
@@ -3885,26 +3892,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="N14:O15"/>
-    <mergeCell ref="P14:P16"/>
-    <mergeCell ref="B33:Z33"/>
-    <mergeCell ref="A9:Z9"/>
-    <mergeCell ref="A10:Z10"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="U13:X13"/>
-    <mergeCell ref="Y13:Y16"/>
-    <mergeCell ref="Z13:Z16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
     <mergeCell ref="B34:Z34"/>
     <mergeCell ref="B35:Z35"/>
     <mergeCell ref="B36:D36"/>
@@ -3921,6 +3908,26 @@
     <mergeCell ref="U14:U16"/>
     <mergeCell ref="V14:V16"/>
     <mergeCell ref="J14:K15"/>
+    <mergeCell ref="A9:Z9"/>
+    <mergeCell ref="A10:Z10"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="Y13:Y16"/>
+    <mergeCell ref="Z13:Z16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="N14:O15"/>
+    <mergeCell ref="P14:P16"/>
+    <mergeCell ref="B33:Z33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>